<commit_message>
Smoothing ranges for same satellites completed
readRINEX was added and it can smooth ranges for epochs that have the same satellites. Need to implement epochs that have fewer/more satellites than the epoch before.
</commit_message>
<xml_diff>
--- a/DOPPLER.xlsx
+++ b/DOPPLER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\UERJ\_Projeto Final\20190115_Marco 91500 IBGE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\UERJ\_Projeto Final\Python\tcc-guilherme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A84783-F74D-4B86-8DBB-5401D22CEE5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A0E987-3FB4-46AA-905C-C038E4F3024B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="6810" xr2:uid="{A6AB510A-5CA1-43AD-ABD2-68ACBD049CAC}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,8 +142,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D982AB-19B5-43BA-A1E8-1E05ED86027B}">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A798" workbookViewId="0">
-      <selection activeCell="B833" sqref="B833"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,8 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.19</v>
+        <f>299792458/1575420000</f>
+        <v>0.19029367279836487</v>
       </c>
       <c r="B2" s="1">
         <v>19</v>
@@ -591,7 +592,7 @@
         <v>-146.63900000000001</v>
       </c>
       <c r="E3" s="2">
-        <f>F3*B3+G3*(0+$A$2*D3)</f>
+        <f>F3*B3+G3*(0-$A$2*D3)</f>
         <v>20716220.958999999</v>
       </c>
       <c r="F3" s="1">
@@ -804,8 +805,8 @@
         <v>-148.19</v>
       </c>
       <c r="E16" s="2">
-        <f>F16*B16+G16*(E3+$A$2*D16)</f>
-        <v>20716243.759094998</v>
+        <f>F16*B16+G16*(E3-$A$2*D16)</f>
+        <v>20716246.576880965</v>
       </c>
       <c r="F16" s="1">
         <f>IF(F3-$A$4 &lt;= $A$4,0.01,F3-$A$4)</f>
@@ -821,11 +822,11 @@
       </c>
       <c r="J16" s="1">
         <f>E16-E3</f>
-        <v>22.800094999372959</v>
+        <v>25.617880966514349</v>
       </c>
       <c r="K16" s="1">
         <f>E16-B16</f>
-        <v>-2.6819050014019012</v>
+        <v>0.1358809657394886</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -987,9 +988,9 @@
       <c r="D29" s="1">
         <v>-149.761</v>
       </c>
-      <c r="E29" s="1">
-        <f>F29*B29+G29*(E16+$A$2*D29)</f>
-        <v>20716269.769350499</v>
+      <c r="E29" s="2">
+        <f>F29*B29+G29*(E16-$A$2*D29)</f>
+        <v>20716275.746445168</v>
       </c>
       <c r="F29" s="1">
         <f>IF(F16-$A$4 &lt;= $A$4,0.01,F16-$A$4)</f>
@@ -1005,11 +1006,11 @@
       </c>
       <c r="J29" s="1">
         <f>E29-E16</f>
-        <v>26.010255500674248</v>
+        <v>29.169564202427864</v>
       </c>
       <c r="K29" s="1">
         <f>E29-B29</f>
-        <v>-6.0516494996845722</v>
+        <v>-7.455483078956604E-2</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1171,9 +1172,9 @@
       <c r="D42" s="1">
         <v>-149.50800000000001</v>
       </c>
-      <c r="E42" s="1">
-        <f>F42*B42+G42*(E29+$A$2*D42)</f>
-        <v>20716284.667074572</v>
+      <c r="E42" s="2">
+        <f>F42*B42+G42*(E29-$A$2*D42)</f>
+        <v>20716294.092180736</v>
       </c>
       <c r="F42" s="1">
         <f>IF(F29-$A$4 &lt;= $A$4,0.01,F29-$A$4)</f>
@@ -1189,11 +1190,11 @@
       </c>
       <c r="J42" s="1">
         <f>E42-E29</f>
-        <v>14.897724073380232</v>
+        <v>18.345735568553209</v>
       </c>
       <c r="K42" s="1">
         <f>E42-B42</f>
-        <v>-7.6419254280626774</v>
+        <v>1.7831807360053062</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1355,9 +1356,9 @@
       <c r="D55" s="1">
         <v>-149.71299999999999</v>
       </c>
-      <c r="E55" s="1">
-        <f>F55*B55+G55*(E42+$A$2*D55)</f>
-        <v>20716319.627520911</v>
+      <c r="E55" s="2">
+        <f>F55*B55+G55*(E42-$A$2*D55)</f>
+        <v>20716332.899523471</v>
       </c>
       <c r="F55" s="1">
         <f>IF(F42-$A$4 &lt;= $A$4,0.01,F42-$A$4)</f>
@@ -1373,11 +1374,11 @@
       </c>
       <c r="J55" s="1">
         <f>E55-E42</f>
-        <v>34.960446339100599</v>
+        <v>38.807342734187841</v>
       </c>
       <c r="K55" s="1">
         <f>E55-B55</f>
-        <v>-15.851479087024927</v>
+        <v>-2.5794765278697014</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -1539,9 +1540,9 @@
       <c r="D68" s="1">
         <v>-149.113</v>
       </c>
-      <c r="E68" s="1">
-        <f>F68*B68+G68*(E55+$A$2*D68)</f>
-        <v>20716339.497762725</v>
+      <c r="E68" s="2">
+        <f>F68*B68+G68*(E55-$A$2*D68)</f>
+        <v>20716356.992445972</v>
       </c>
       <c r="F68" s="1">
         <f>IF(F55-$A$4 &lt;= $A$4,0.01,F55-$A$4)</f>
@@ -1557,11 +1558,11 @@
       </c>
       <c r="J68" s="1">
         <f>E68-E55</f>
-        <v>19.870241813361645</v>
+        <v>24.092922501266003</v>
       </c>
       <c r="K68" s="1">
         <f>E68-B68</f>
-        <v>-16.06723727658391</v>
+        <v>1.4274459704756737</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -1723,9 +1724,9 @@
       <c r="D81" s="1">
         <v>-149.69499999999999</v>
       </c>
-      <c r="E81" s="1">
-        <f>F81*B81+G81*(E68+$A$2*D81)</f>
-        <v>20716355.643113814</v>
+      <c r="E81" s="2">
+        <f>F81*B81+G81*(E68-$A$2*D81)</f>
+        <v>20716377.96993719</v>
       </c>
       <c r="F81" s="1">
         <f>IF(F68-$A$4 &lt;= $A$4,0.01,F68-$A$4)</f>
@@ -1741,11 +1742,11 @@
       </c>
       <c r="J81" s="1">
         <f>E81-E68</f>
-        <v>16.145351089537144</v>
+        <v>20.977491218596697</v>
       </c>
       <c r="K81" s="1">
         <f>E81-B81</f>
-        <v>-19.108886186033487</v>
+        <v>3.2179371900856495</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -1907,9 +1908,9 @@
       <c r="D94" s="1">
         <v>-151.12299999999999</v>
       </c>
-      <c r="E94" s="1">
-        <f>F94*B94+G94*(E81+$A$2*D94)</f>
-        <v>20716377.695560329</v>
+      <c r="E94" s="2">
+        <f>F94*B94+G94*(E81-$A$2*D94)</f>
+        <v>20716405.624840759</v>
       </c>
       <c r="F94" s="1">
         <f>IF(F81-$A$4 &lt;= $A$4,0.01,F81-$A$4)</f>
@@ -1925,11 +1926,11 @@
       </c>
       <c r="J94" s="1">
         <f>E94-E81</f>
-        <v>22.052446514368057</v>
+        <v>27.654903568327427</v>
       </c>
       <c r="K94" s="1">
         <f>E94-B94</f>
-        <v>-27.335439670830965</v>
+        <v>0.59384075924754143</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -2091,9 +2092,9 @@
       <c r="D107" s="1">
         <v>-152.16999999999999</v>
       </c>
-      <c r="E107" s="1">
-        <f>F107*B107+G107*(E94+$A$2*D107)</f>
-        <v>20716403.93750412</v>
+      <c r="E107" s="2">
+        <f>F107*B107+G107*(E94-$A$2*D107)</f>
+        <v>20716438.256931569</v>
       </c>
       <c r="F107" s="1">
         <f>IF(F94-$A$4 &lt;= $A$4,0.01,F94-$A$4)</f>
@@ -2109,11 +2110,11 @@
       </c>
       <c r="J107" s="1">
         <f>E107-E94</f>
-        <v>26.241943791508675</v>
+        <v>32.63209081068635</v>
       </c>
       <c r="K107" s="1">
         <f>E107-B107</f>
-        <v>-36.769495878368616</v>
+        <v>-2.4500684291124344</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -2275,9 +2276,9 @@
       <c r="D120" s="1">
         <v>-152.61699999999999</v>
       </c>
-      <c r="E120" s="1">
-        <f>F120*B120+G120*(E107+$A$2*D120)</f>
-        <v>20716422.983723342</v>
+      <c r="E120" s="2">
+        <f>F120*B120+G120*(E107-$A$2*D120)</f>
+        <v>20716464.545141451</v>
       </c>
       <c r="F120" s="1">
         <f>IF(F107-$A$4 &lt;= $A$4,0.01,F107-$A$4)</f>
@@ -2293,11 +2294,11 @@
       </c>
       <c r="J120" s="1">
         <f>E120-E107</f>
-        <v>19.046219222247601</v>
+        <v>26.28820988163352</v>
       </c>
       <c r="K120" s="1">
         <f>E120-B120</f>
-        <v>-39.308276657015085</v>
+        <v>2.2531414516270161</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -2459,9 +2460,9 @@
       <c r="D133" s="1">
         <v>-153.28899999999999</v>
       </c>
-      <c r="E133" s="1">
-        <f>F133*B133+G133*(E120+$A$2*D133)</f>
-        <v>20716449.95990666</v>
+      <c r="E133" s="2">
+        <f>F133*B133+G133*(E120-$A$2*D133)</f>
+        <v>20716499.88803412</v>
       </c>
       <c r="F133" s="1">
         <f>IF(F120-$A$4 &lt;= $A$4,0.01,F120-$A$4)</f>
@@ -2477,11 +2478,11 @@
       </c>
       <c r="J133" s="1">
         <f>E133-E120</f>
-        <v>26.976183317601681</v>
+        <v>35.342892669141293</v>
       </c>
       <c r="K133" s="1">
         <f>E133-B133</f>
-        <v>-56.101093340665102</v>
+        <v>-6.1729658804833889</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
@@ -2643,9 +2644,9 @@
       <c r="D146" s="1">
         <v>-152.37100000000001</v>
       </c>
-      <c r="E146" s="1">
-        <f>F146*B146+G146*(E133+$A$2*D146)</f>
-        <v>20716467.64677915</v>
+      <c r="E146" s="2">
+        <f>F146*B146+G146*(E133-$A$2*D146)</f>
+        <v>20716526.977399223</v>
       </c>
       <c r="F146" s="1">
         <f>IF(F133-$A$4 &lt;= $A$4,0.01,F133-$A$4)</f>
@@ -2661,11 +2662,11 @@
       </c>
       <c r="J146" s="1">
         <f>E146-E133</f>
-        <v>17.686872489750385</v>
+        <v>27.089365102350712</v>
       </c>
       <c r="K146" s="1">
         <f>E146-B146</f>
-        <v>-57.001220848411322</v>
+        <v>2.329399224370718</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
@@ -2827,9 +2828,9 @@
       <c r="D159" s="1">
         <v>-153.46</v>
       </c>
-      <c r="E159" s="1">
-        <f>F159*B159+G159*(E146+$A$2*D159)</f>
-        <v>20716485.06442748</v>
+      <c r="E159" s="2">
+        <f>F159*B159+G159*(E146-$A$2*D159)</f>
+        <v>20716555.678719744</v>
       </c>
       <c r="F159" s="1">
         <f>IF(F146-$A$4 &lt;= $A$4,0.01,F146-$A$4)</f>
@@ -2845,11 +2846,11 @@
       </c>
       <c r="J159" s="1">
         <f>E159-E146</f>
-        <v>17.417648330330849</v>
+        <v>28.701320521533489</v>
       </c>
       <c r="K159" s="1">
         <f>E159-B159</f>
-        <v>-69.862572520971298</v>
+        <v>0.75171974301338196</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
@@ -3011,9 +3012,9 @@
       <c r="D172" s="1">
         <v>-154.631</v>
       </c>
-      <c r="E172" s="1">
-        <f>F172*B172+G172*(E159+$A$2*D172)</f>
-        <v>20716501.961699359</v>
+      <c r="E172" s="2">
+        <f>F172*B172+G172*(E159-$A$2*D172)</f>
+        <v>20716586.084363423</v>
       </c>
       <c r="F172" s="1">
         <f>IF(F159-$A$4 &lt;= $A$4,0.01,F159-$A$4)</f>
@@ -3029,11 +3030,11 @@
       </c>
       <c r="J172" s="1">
         <f>E172-E159</f>
-        <v>16.897271879017353</v>
+        <v>30.405643679201603</v>
       </c>
       <c r="K172" s="1">
         <f>E172-B172</f>
-        <v>-85.943300642073154</v>
+        <v>-1.8206365779042244</v>
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
@@ -3195,9 +3196,9 @@
       <c r="D185" s="1">
         <v>-156.441</v>
       </c>
-      <c r="E185" s="1">
-        <f>F185*B185+G185*(E172+$A$2*D185)</f>
-        <v>20716519.979036544</v>
+      <c r="E185" s="2">
+        <f>F185*B185+G185*(E172-$A$2*D185)</f>
+        <v>20716620.510367118</v>
       </c>
       <c r="F185" s="1">
         <f>IF(F172-$A$4 &lt;= $A$4,0.01,F172-$A$4)</f>
@@ -3213,11 +3214,11 @@
       </c>
       <c r="J185" s="1">
         <f>E185-E172</f>
-        <v>18.017337184399366</v>
+        <v>34.426003694534302</v>
       </c>
       <c r="K185" s="1">
         <f>E185-B185</f>
-        <v>-111.3959634564817</v>
+        <v>-10.86463288217783</v>
       </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
@@ -3379,9 +3380,9 @@
       <c r="D198" s="1">
         <v>-158.16</v>
       </c>
-      <c r="E198" s="1">
-        <f>F198*B198+G198*(E185+$A$2*D198)</f>
-        <v>20716530.986227404</v>
+      <c r="E198" s="2">
+        <f>F198*B198+G198*(E185-$A$2*D198)</f>
+        <v>20716651.495160799</v>
       </c>
       <c r="F198" s="1">
         <f>IF(F185-$A$4 &lt;= $A$4,0.01,F185-$A$4)</f>
@@ -3397,11 +3398,11 @@
       </c>
       <c r="J198" s="1">
         <f>E198-E185</f>
-        <v>11.007190860807896</v>
+        <v>30.984793681651354</v>
       </c>
       <c r="K198" s="1">
         <f>E198-B198</f>
-        <v>-123.17277259752154</v>
+        <v>-2.6638392023742199</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
@@ -3563,9 +3564,9 @@
       <c r="D211" s="1">
         <v>-159.03</v>
       </c>
-      <c r="E211" s="1">
-        <f>F211*B211+G211*(E198+$A$2*D211)</f>
-        <v>20716535.40542192</v>
+      <c r="E211" s="2">
+        <f>F211*B211+G211*(E198-$A$2*D211)</f>
+        <v>20716680.195050865</v>
       </c>
       <c r="F211" s="1">
         <f>IF(F198-$A$4 &lt;= $A$4,0.01,F198-$A$4)</f>
@@ -3581,11 +3582,11 @@
       </c>
       <c r="J211" s="1">
         <f>E211-E198</f>
-        <v>4.4191945157945156</v>
+        <v>28.699890065938234</v>
       </c>
       <c r="K211" s="1">
         <f>E211-B211</f>
-        <v>-138.53957808017731</v>
+        <v>6.2500508651137352</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
@@ -3747,9 +3748,9 @@
       <c r="D224" s="1">
         <v>-159.50200000000001</v>
       </c>
-      <c r="E224" s="1">
-        <f>F224*B224+G224*(E211+$A$2*D224)</f>
-        <v>20716534.518935628</v>
+      <c r="E224" s="2">
+        <f>F224*B224+G224*(E211-$A$2*D224)</f>
+        <v>20716709.149081424</v>
       </c>
       <c r="F224" s="1">
         <f>IF(F211-$A$4 &lt;= $A$4,0.01,F211-$A$4)</f>
@@ -3765,11 +3766,11 @@
       </c>
       <c r="J224" s="1">
         <f>E224-E211</f>
-        <v>-0.88648629188537598</v>
+        <v>28.954030558466911</v>
       </c>
       <c r="K224" s="1">
         <f>E224-B224</f>
-        <v>-166.70706437155604</v>
+        <v>7.923081424087286</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
@@ -3931,9 +3932,9 @@
       <c r="D237" s="1">
         <v>-158.66800000000001</v>
       </c>
-      <c r="E237" s="1">
-        <f>F237*B237+G237*(E224+$A$2*D237)</f>
-        <v>20716525.946114063</v>
+      <c r="E237" s="2">
+        <f>F237*B237+G237*(E224-$A$2*D237)</f>
+        <v>20716737.419638108</v>
       </c>
       <c r="F237" s="1">
         <f>IF(F224-$A$4 &lt;= $A$4,0.01,F224-$A$4)</f>
@@ -3949,11 +3950,11 @@
       </c>
       <c r="J237" s="1">
         <f>E237-E224</f>
-        <v>-8.5728215649724007</v>
+        <v>28.270556684583426</v>
       </c>
       <c r="K237" s="1">
         <f>E237-B237</f>
-        <v>-194.1668859384954</v>
+        <v>17.306638106703758</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
@@ -4115,9 +4116,9 @@
       <c r="D250" s="1">
         <v>-159.108</v>
       </c>
-      <c r="E250" s="1">
-        <f>F250*B250+G250*(E237+$A$2*D250)</f>
-        <v>20716498.337308124</v>
+      <c r="E250" s="2">
+        <f>F250*B250+G250*(E237-$A$2*D250)</f>
+        <v>20716767.598784961</v>
       </c>
       <c r="F250" s="1">
         <f>IF(F237-$A$4 &lt;= $A$4,0.01,F237-$A$4)</f>
@@ -4133,11 +4134,11 @@
       </c>
       <c r="J250" s="1">
         <f>E250-E237</f>
-        <v>-27.608805939555168</v>
+        <v>30.179146852344275</v>
       </c>
       <c r="K250" s="1">
         <f>E250-B250</f>
-        <v>-259.54969187453389</v>
+        <v>9.7117849625647068</v>
       </c>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.25">
@@ -4300,9 +4301,9 @@
       <c r="D263" s="1">
         <v>-160.137</v>
       </c>
-      <c r="E263" s="1">
-        <f>F263*B263+G263*(E250+$A$2*D263)</f>
-        <v>20716471.200765345</v>
+      <c r="E263" s="2">
+        <f>F263*B263+G263*(E250-$A$2*D263)</f>
+        <v>20716798.059724413</v>
       </c>
       <c r="F263" s="1">
         <f>IF(F250-$A$4 &lt;= $A$4,0.01,F250-$A$4)</f>
@@ -4318,11 +4319,11 @@
       </c>
       <c r="J263" s="1">
         <f>E263-E250</f>
-        <v>-27.136542778462172</v>
+        <v>30.460939452052116</v>
       </c>
       <c r="K263" s="1">
         <f>E263-B263</f>
-        <v>-325.65923465415835</v>
+        <v>1.1997244134545326</v>
       </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
@@ -4484,9 +4485,9 @@
       <c r="D276" s="1">
         <v>-160.845</v>
       </c>
-      <c r="E276" s="1">
-        <f>F276*B276+G276*(E263+$A$2*D276)</f>
-        <v>20716444.454243194</v>
+      <c r="E276" s="2">
+        <f>F276*B276+G276*(E263-$A$2*D276)</f>
+        <v>20716828.601265114</v>
       </c>
       <c r="F276" s="1">
         <f>IF(F263-$A$4 &lt;= $A$4,0.01,F263-$A$4)</f>
@@ -4502,11 +4503,11 @@
       </c>
       <c r="J276" s="1">
         <f>E276-E263</f>
-        <v>-26.746522150933743</v>
+        <v>30.541540700942278</v>
       </c>
       <c r="K276" s="1">
         <f>E276-B276</f>
-        <v>-377.58875680714846</v>
+        <v>6.5582651123404503</v>
       </c>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.25">
@@ -4668,9 +4669,9 @@
       <c r="D289" s="1">
         <v>-162.05099999999999</v>
       </c>
-      <c r="E289" s="1">
-        <f>F289*B289+G289*(E276+$A$2*D289)</f>
-        <v>20716418.108087663</v>
+      <c r="E289" s="2">
+        <f>F289*B289+G289*(E276-$A$2*D289)</f>
+        <v>20716859.424339633</v>
       </c>
       <c r="F289" s="1">
         <f>IF(F276-$A$4 &lt;= $A$4,0.01,F276-$A$4)</f>
@@ -4686,11 +4687,11 @@
       </c>
       <c r="J289" s="1">
         <f>E289-E276</f>
-        <v>-26.346155531704426</v>
+        <v>30.823074519634247</v>
       </c>
       <c r="K289" s="1">
         <f>E289-B289</f>
-        <v>-439.90991233661771</v>
+        <v>1.4063396342098713</v>
       </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.25">
@@ -4852,9 +4853,9 @@
       <c r="D302" s="1">
         <v>-163.28899999999999</v>
       </c>
-      <c r="E302" s="1">
-        <f>F302*B302+G302*(E289+$A$2*D302)</f>
-        <v>20716392.149275888</v>
+      <c r="E302" s="2">
+        <f>F302*B302+G302*(E289-$A$2*D302)</f>
+        <v>20716890.52916114</v>
       </c>
       <c r="F302" s="1">
         <f>IF(F289-$A$4 &lt;= $A$4,0.01,F289-$A$4)</f>
@@ -4870,11 +4871,11 @@
       </c>
       <c r="J302" s="1">
         <f>E302-E289</f>
-        <v>-25.958811774849892</v>
+        <v>31.104821506887674</v>
       </c>
       <c r="K302" s="1">
         <f>E302-B302</f>
-        <v>-501.54372411221266</v>
+        <v>-3.1638388596475124</v>
       </c>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.25">
@@ -5036,9 +5037,9 @@
       <c r="D315" s="1">
         <v>-163.43799999999999</v>
       </c>
-      <c r="E315" s="1">
-        <f>F315*B315+G315*(E302+$A$2*D315)</f>
-        <v>20716366.66785533</v>
+      <c r="E315" s="2">
+        <f>F315*B315+G315*(E302-$A$2*D315)</f>
+        <v>20716921.596834652</v>
       </c>
       <c r="F315" s="1">
         <f>IF(F302-$A$4 &lt;= $A$4,0.01,F302-$A$4)</f>
@@ -5054,11 +5055,11 @@
       </c>
       <c r="J315" s="1">
         <f>E315-E302</f>
-        <v>-25.481420557945967</v>
+        <v>31.06767351180315</v>
       </c>
       <c r="K315" s="1">
         <f>E315-B315</f>
-        <v>-551.60814467072487</v>
+        <v>3.3208346515893936</v>
       </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
@@ -5220,9 +5221,9 @@
       <c r="D328" s="1">
         <v>-163.249</v>
       </c>
-      <c r="E328" s="1">
-        <f>F328*B328+G328*(E315+$A$2*D328)</f>
-        <v>20716341.794579875</v>
+      <c r="E328" s="2">
+        <f>F328*B328+G328*(E315-$A$2*D328)</f>
+        <v>20716952.636005577</v>
       </c>
       <c r="F328" s="1">
         <f>IF(F315-$A$4 &lt;= $A$4,0.01,F315-$A$4)</f>
@@ -5238,11 +5239,11 @@
       </c>
       <c r="J328" s="1">
         <f>E328-E315</f>
-        <v>-24.873275455087423</v>
+        <v>31.039170924574137</v>
       </c>
       <c r="K328" s="1">
         <f>E328-B328</f>
-        <v>-608.25942012667656</v>
+        <v>2.582005575299263</v>
       </c>
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.25">
@@ -5404,9 +5405,9 @@
       <c r="D341" s="1">
         <v>-164.09800000000001</v>
       </c>
-      <c r="E341" s="1">
-        <f>F341*B341+G341*(E328+$A$2*D341)</f>
-        <v>20716317.238180276</v>
+      <c r="E341" s="2">
+        <f>F341*B341+G341*(E328-$A$2*D341)</f>
+        <v>20716983.752568528</v>
       </c>
       <c r="F341" s="1">
         <f>IF(F328-$A$4 &lt;= $A$4,0.01,F328-$A$4)</f>
@@ -5422,11 +5423,11 @@
       </c>
       <c r="J341" s="1">
         <f>E341-E328</f>
-        <v>-24.55639959871769</v>
+        <v>31.116562951356173</v>
       </c>
       <c r="K341" s="1">
         <f>E341-B341</f>
-        <v>-655.5998197235167</v>
+        <v>10.914568528532982</v>
       </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
@@ -5588,9 +5589,9 @@
       <c r="D354" s="1">
         <v>-163.99100000000001</v>
       </c>
-      <c r="E354" s="1">
-        <f>F354*B354+G354*(E341+$A$2*D354)</f>
-        <v>20716293.292231373</v>
+      <c r="E354" s="2">
+        <f>F354*B354+G354*(E341-$A$2*D354)</f>
+        <v>20717014.882568039</v>
       </c>
       <c r="F354" s="1">
         <f>IF(F341-$A$4 &lt;= $A$4,0.01,F341-$A$4)</f>
@@ -5606,11 +5607,11 @@
       </c>
       <c r="J354" s="1">
         <f>E354-E341</f>
-        <v>-23.945948902517557</v>
+        <v>31.12999951094389</v>
       </c>
       <c r="K354" s="1">
         <f>E354-B354</f>
-        <v>-714.02176862582564</v>
+        <v>7.5685680396854877</v>
       </c>
     </row>
     <row r="355" spans="1:11" x14ac:dyDescent="0.25">
@@ -5772,9 +5773,9 @@
       <c r="D367" s="1">
         <v>-164.31200000000001</v>
       </c>
-      <c r="E367" s="1">
-        <f>F367*B367+G367*(E354+$A$2*D367)</f>
-        <v>20716269.822161861</v>
+      <c r="E367" s="2">
+        <f>F367*B367+G367*(E354-$A$2*D367)</f>
+        <v>20717046.058540985</v>
       </c>
       <c r="F367" s="1">
         <f>IF(F354-$A$4 &lt;= $A$4,0.01,F354-$A$4)</f>
@@ -5790,11 +5791,11 @@
       </c>
       <c r="J367" s="1">
         <f>E367-E354</f>
-        <v>-23.470069512724876</v>
+        <v>31.175972945988178</v>
       </c>
       <c r="K367" s="1">
         <f>E367-B367</f>
-        <v>-767.1718381382525</v>
+        <v>9.0645409859716892</v>
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.25">
@@ -5956,9 +5957,9 @@
       <c r="D380" s="1">
         <v>-164.61799999999999</v>
       </c>
-      <c r="E380" s="1">
-        <f>F380*B380+G380*(E367+$A$2*D380)</f>
-        <v>20716246.870994441</v>
+      <c r="E380" s="2">
+        <f>F380*B380+G380*(E367-$A$2*D380)</f>
+        <v>20717077.322161764</v>
       </c>
       <c r="F380" s="1">
         <f>IF(F367-$A$4 &lt;= $A$4,0.01,F367-$A$4)</f>
@@ -5974,11 +5975,11 @@
       </c>
       <c r="J380" s="1">
         <f>E380-E367</f>
-        <v>-22.951167419552803</v>
+        <v>31.263620778918266</v>
       </c>
       <c r="K380" s="1">
         <f>E380-B380</f>
-        <v>-824.29900556057692</v>
+        <v>6.1521617621183395</v>
       </c>
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.25">
@@ -6140,9 +6141,9 @@
       <c r="D393" s="1">
         <v>-165.66399999999999</v>
       </c>
-      <c r="E393" s="1">
-        <f>F393*B393+G393*(E380+$A$2*D393)</f>
-        <v>20716224.357306097</v>
+      <c r="E393" s="2">
+        <f>F393*B393+G393*(E380-$A$2*D393)</f>
+        <v>20717108.874923047</v>
       </c>
       <c r="F393" s="1">
         <f>IF(F380-$A$4 &lt;= $A$4,0.01,F380-$A$4)</f>
@@ -6158,11 +6159,11 @@
       </c>
       <c r="J393" s="1">
         <f>E393-E380</f>
-        <v>-22.51368834450841</v>
+        <v>31.552761282771826</v>
       </c>
       <c r="K393" s="1">
         <f>E393-B393</f>
-        <v>-887.28469390422106</v>
+        <v>-2.7670769542455673</v>
       </c>
     </row>
     <row r="394" spans="1:11" x14ac:dyDescent="0.25">
@@ -6324,9 +6325,9 @@
       <c r="D406" s="1">
         <v>-166.56200000000001</v>
       </c>
-      <c r="E406" s="1">
-        <f>F406*B406+G406*(E393+$A$2*D406)</f>
-        <v>20716202.223620836</v>
+      <c r="E406" s="2">
+        <f>F406*B406+G406*(E393-$A$2*D406)</f>
+        <v>20717140.605111599</v>
       </c>
       <c r="F406" s="1">
         <f>IF(F393-$A$4 &lt;= $A$4,0.01,F393-$A$4)</f>
@@ -6342,11 +6343,11 @@
       </c>
       <c r="J406" s="1">
         <f>E406-E393</f>
-        <v>-22.133685261011124</v>
+        <v>31.730188552290201</v>
       </c>
       <c r="K406" s="1">
         <f>E406-B406</f>
-        <v>-941.79637916386127</v>
+        <v>-3.4148884005844593</v>
       </c>
     </row>
     <row r="407" spans="1:11" x14ac:dyDescent="0.25">
@@ -6508,9 +6509,9 @@
       <c r="D419" s="1">
         <v>-168.715</v>
       </c>
-      <c r="E419" s="1">
-        <f>F419*B419+G419*(E406+$A$2*D419)</f>
-        <v>20716180.239063125</v>
+      <c r="E419" s="2">
+        <f>F419*B419+G419*(E406-$A$2*D419)</f>
+        <v>20717172.756373517</v>
       </c>
       <c r="F419" s="1">
         <f>IF(F406-$A$4 &lt;= $A$4,0.01,F406-$A$4)</f>
@@ -6526,11 +6527,11 @@
       </c>
       <c r="J419" s="1">
         <f>E419-E406</f>
-        <v>-21.984557710587978</v>
+        <v>32.151261918246746</v>
       </c>
       <c r="K419" s="1">
         <f>E419-B419</f>
-        <v>-997.05793687328696</v>
+        <v>-4.5406264811754227</v>
       </c>
     </row>
     <row r="420" spans="1:11" x14ac:dyDescent="0.25">
@@ -6692,9 +6693,9 @@
       <c r="D432" s="1">
         <v>-169.083</v>
       </c>
-      <c r="E432" s="1">
-        <f>F432*B432+G432*(E419+$A$2*D432)</f>
-        <v>20716158.677940194</v>
+      <c r="E432" s="2">
+        <f>F432*B432+G432*(E419-$A$2*D432)</f>
+        <v>20717204.92826061</v>
       </c>
       <c r="F432" s="1">
         <f>IF(F419-$A$4 &lt;= $A$4,0.01,F419-$A$4)</f>
@@ -6710,11 +6711,11 @@
       </c>
       <c r="J432" s="1">
         <f>E432-E419</f>
-        <v>-21.561122931540012</v>
+        <v>32.171887092292309</v>
       </c>
       <c r="K432" s="1">
         <f>E432-B432</f>
-        <v>-1045.9000598080456</v>
+        <v>0.35026060789823532</v>
       </c>
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.25">
@@ -6876,9 +6877,9 @@
       <c r="D445" s="1">
         <v>-170.41</v>
       </c>
-      <c r="E445" s="1">
-        <f>F445*B445+G445*(E432+$A$2*D445)</f>
-        <v>20716137.37960979</v>
+      <c r="E445" s="2">
+        <f>F445*B445+G445*(E432-$A$2*D445)</f>
+        <v>20717237.325213339</v>
       </c>
       <c r="F445" s="1">
         <f>IF(F432-$A$4 &lt;= $A$4,0.01,F432-$A$4)</f>
@@ -6894,11 +6895,11 @@
       </c>
       <c r="J445" s="1">
         <f>E445-E432</f>
-        <v>-21.298330403864384</v>
+        <v>32.396952729672194</v>
       </c>
       <c r="K445" s="1">
         <f>E445-B445</f>
-        <v>-1096.8773902095854</v>
+        <v>3.06821333989501</v>
       </c>
     </row>
     <row r="446" spans="1:11" x14ac:dyDescent="0.25">
@@ -7060,9 +7061,9 @@
       <c r="D458" s="1">
         <v>-170.23</v>
       </c>
-      <c r="E458" s="1">
-        <f>F458*B458+G458*(E445+$A$2*D458)</f>
-        <v>20716116.720850695</v>
+      <c r="E458" s="2">
+        <f>F458*B458+G458*(E445-$A$2*D458)</f>
+        <v>20717269.757016208</v>
       </c>
       <c r="F458" s="1">
         <f>IF(F445-$A$4 &lt;= $A$4,0.01,F445-$A$4)</f>
@@ -7078,11 +7079,11 @@
       </c>
       <c r="J458" s="1">
         <f>E458-E445</f>
-        <v>-20.658759094774723</v>
+        <v>32.431802868843079</v>
       </c>
       <c r="K458" s="1">
         <f>E458-B458</f>
-        <v>-1156.8091493062675</v>
+        <v>-3.77298379316926</v>
       </c>
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.25">
@@ -7244,9 +7245,9 @@
       <c r="D471" s="1">
         <v>-170.54</v>
       </c>
-      <c r="E471" s="1">
-        <f>F471*B471+G471*(E458+$A$2*D471)</f>
-        <v>20716096.411228184</v>
+      <c r="E471" s="2">
+        <f>F471*B471+G471*(E458-$A$2*D471)</f>
+        <v>20717302.123762175</v>
       </c>
       <c r="F471" s="1">
         <f>IF(F458-$A$4 &lt;= $A$4,0.01,F458-$A$4)</f>
@@ -7262,11 +7263,11 @@
       </c>
       <c r="J471" s="1">
         <f>E471-E458</f>
-        <v>-20.309622511267662</v>
+        <v>32.366745967417955</v>
       </c>
       <c r="K471" s="1">
         <f>E471-B471</f>
-        <v>-1197.2047718167305</v>
+        <v>8.5077621750533581</v>
       </c>
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.25">
@@ -7428,9 +7429,9 @@
       <c r="D484" s="1">
         <v>-172.178</v>
       </c>
-      <c r="E484" s="1">
-        <f>F484*B484+G484*(E471+$A$2*D484)</f>
-        <v>20716076.506244104</v>
+      <c r="E484" s="2">
+        <f>F484*B484+G484*(E471-$A$2*D484)</f>
+        <v>20717334.98507471</v>
       </c>
       <c r="F484" s="1">
         <f>IF(F471-$A$4 &lt;= $A$4,0.01,F471-$A$4)</f>
@@ -7446,11 +7447,11 @@
       </c>
       <c r="J484" s="1">
         <f>E484-E471</f>
-        <v>-19.904984079301357</v>
+        <v>32.861312534660101</v>
       </c>
       <c r="K484" s="1">
         <f>E484-B484</f>
-        <v>-1268.0747558958828</v>
+        <v>-9.5959252901375294</v>
       </c>
     </row>
     <row r="485" spans="1:11" x14ac:dyDescent="0.25">
@@ -7612,9 +7613,9 @@
       <c r="D497" s="1">
         <v>-172.55</v>
       </c>
-      <c r="E497" s="1">
-        <f>F497*B497+G497*(E484+$A$2*D497)</f>
-        <v>20716056.931196664</v>
+      <c r="E497" s="2">
+        <f>F497*B497+G497*(E484-$A$2*D497)</f>
+        <v>20717367.788715471</v>
       </c>
       <c r="F497" s="1">
         <f>IF(F484-$A$4 &lt;= $A$4,0.01,F484-$A$4)</f>
@@ -7630,11 +7631,11 @@
       </c>
       <c r="J497" s="1">
         <f>E497-E484</f>
-        <v>-19.575047440826893</v>
+        <v>32.803640760481358</v>
       </c>
       <c r="K497" s="1">
         <f>E497-B497</f>
-        <v>-1307.7358033359051</v>
+        <v>3.1217154711484909</v>
       </c>
     </row>
     <row r="498" spans="1:11" x14ac:dyDescent="0.25">
@@ -7796,9 +7797,9 @@
       <c r="D510" s="1">
         <v>-172.46100000000001</v>
       </c>
-      <c r="E510" s="1">
-        <f>F510*B510+G510*(E497+$A$2*D510)</f>
-        <v>20716038.012330595</v>
+      <c r="E510" s="2">
+        <f>F510*B510+G510*(E497-$A$2*D510)</f>
+        <v>20717400.691243049</v>
       </c>
       <c r="F510" s="1">
         <f>IF(F497-$A$4 &lt;= $A$4,0.01,F497-$A$4)</f>
@@ -7814,11 +7815,11 @@
       </c>
       <c r="J510" s="1">
         <f>E510-E497</f>
-        <v>-18.918866068124771</v>
+        <v>32.902527578175068</v>
       </c>
       <c r="K510" s="1">
         <f>E510-B510</f>
-        <v>-1371.0236694030464</v>
+        <v>-8.3447569496929646</v>
       </c>
     </row>
     <row r="511" spans="1:11" x14ac:dyDescent="0.25">
@@ -7980,9 +7981,9 @@
       <c r="D523" s="1">
         <v>-172.274</v>
       </c>
-      <c r="E523" s="1">
-        <f>F523*B523+G523*(E510+$A$2*D523)</f>
-        <v>20716019.641607892</v>
+      <c r="E523" s="2">
+        <f>F523*B523+G523*(E510-$A$2*D523)</f>
+        <v>20717433.553296287</v>
       </c>
       <c r="F523" s="1">
         <f>IF(F510-$A$4 &lt;= $A$4,0.01,F510-$A$4)</f>
@@ -7998,11 +7999,11 @@
       </c>
       <c r="J523" s="1">
         <f>E523-E510</f>
-        <v>-18.370722703635693</v>
+        <v>32.862053237855434</v>
       </c>
       <c r="K523" s="1">
         <f>E523-B523</f>
-        <v>-1421.7723921090364</v>
+        <v>-7.8607037141919136</v>
       </c>
     </row>
     <row r="524" spans="1:11" x14ac:dyDescent="0.25">
@@ -8164,9 +8165,9 @@
       <c r="D536" s="1">
         <v>-173.779</v>
       </c>
-      <c r="E536" s="1">
-        <f>F536*B536+G536*(E523+$A$2*D536)</f>
-        <v>20716001.444311909</v>
+      <c r="E536" s="2">
+        <f>F536*B536+G536*(E523-$A$2*D536)</f>
+        <v>20717466.643067047</v>
       </c>
       <c r="F536" s="1">
         <f>IF(F523-$A$4 &lt;= $A$4,0.01,F523-$A$4)</f>
@@ -8182,11 +8183,11 @@
       </c>
       <c r="J536" s="1">
         <f>E536-E523</f>
-        <v>-18.197295982390642</v>
+        <v>33.089770760387182</v>
       </c>
       <c r="K536" s="1">
         <f>E536-B536</f>
-        <v>-1467.2506880909204</v>
+        <v>-2.0519329532980919</v>
       </c>
     </row>
     <row r="537" spans="1:11" x14ac:dyDescent="0.25">
@@ -8348,9 +8349,9 @@
       <c r="D549" s="1">
         <v>-174.45099999999999</v>
       </c>
-      <c r="E549" s="1">
-        <f>F549*B549+G549*(E536+$A$2*D549)</f>
-        <v>20715983.695315689</v>
+      <c r="E549" s="2">
+        <f>F549*B549+G549*(E536-$A$2*D549)</f>
+        <v>20717499.921268672</v>
       </c>
       <c r="F549" s="1">
         <f>IF(F536-$A$4 &lt;= $A$4,0.01,F536-$A$4)</f>
@@ -8366,11 +8367,11 @@
       </c>
       <c r="J549" s="1">
         <f>E549-E536</f>
-        <v>-17.748996220529079</v>
+        <v>33.278201624751091</v>
       </c>
       <c r="K549" s="1">
         <f>E549-B549</f>
-        <v>-1524.2726843096316</v>
+        <v>-8.0467313267290592</v>
       </c>
     </row>
     <row r="550" spans="1:11" x14ac:dyDescent="0.25">
@@ -8532,9 +8533,9 @@
       <c r="D562" s="1">
         <v>-174.203</v>
       </c>
-      <c r="E562" s="1">
-        <f>F562*B562+G562*(E549+$A$2*D562)</f>
-        <v>20715966.506218232</v>
+      <c r="E562" s="2">
+        <f>F562*B562+G562*(E549-$A$2*D562)</f>
+        <v>20717533.155727379</v>
       </c>
       <c r="F562" s="1">
         <f>IF(F549-$A$4 &lt;= $A$4,0.01,F549-$A$4)</f>
@@ -8550,11 +8551,11 @@
       </c>
       <c r="J562" s="1">
         <f>E562-E549</f>
-        <v>-17.189097456634045</v>
+        <v>33.234458707273006</v>
       </c>
       <c r="K562" s="1">
         <f>E562-B562</f>
-        <v>-1575.0377817675471</v>
+        <v>-8.3882726207375526</v>
       </c>
     </row>
     <row r="563" spans="1:11" x14ac:dyDescent="0.25">
@@ -8716,9 +8717,9 @@
       <c r="D575" s="1">
         <v>-175.22900000000001</v>
       </c>
-      <c r="E575" s="1">
-        <f>F575*B575+G575*(E562+$A$2*D575)</f>
-        <v>20715949.679761149</v>
+      <c r="E575" s="2">
+        <f>F575*B575+G575*(E562-$A$2*D575)</f>
+        <v>20717566.634870399</v>
       </c>
       <c r="F575" s="1">
         <f>IF(F562-$A$4 &lt;= $A$4,0.01,F562-$A$4)</f>
@@ -8734,11 +8735,11 @@
       </c>
       <c r="J575" s="1">
         <f>E575-E562</f>
-        <v>-16.82645708322525</v>
+        <v>33.479143019765615</v>
       </c>
       <c r="K575" s="1">
         <f>E575-B575</f>
-        <v>-1630.2382388524711</v>
+        <v>-13.28312960267067</v>
       </c>
     </row>
     <row r="576" spans="1:11" x14ac:dyDescent="0.25">
@@ -8900,9 +8901,9 @@
       <c r="D588" s="1">
         <v>-175.8</v>
       </c>
-      <c r="E588" s="1">
-        <f>F588*B588+G588*(E575+$A$2*D588)</f>
-        <v>20715933.210953541</v>
+      <c r="E588" s="2">
+        <f>F588*B588+G588*(E575-$A$2*D588)</f>
+        <v>20717600.183583099</v>
       </c>
       <c r="F588" s="1">
         <f>IF(F575-$A$4 &lt;= $A$4,0.01,F575-$A$4)</f>
@@ -8918,11 +8919,11 @@
       </c>
       <c r="J588" s="1">
         <f>E588-E575</f>
-        <v>-16.468807607889175</v>
+        <v>33.548712700605392</v>
       </c>
       <c r="K588" s="1">
         <f>E588-B588</f>
-        <v>-1676.3860464580357</v>
+        <v>-9.413416899740696</v>
       </c>
     </row>
     <row r="589" spans="1:11" x14ac:dyDescent="0.25">
@@ -9084,9 +9085,9 @@
       <c r="D601" s="1">
         <v>-177.99600000000001</v>
       </c>
-      <c r="E601" s="1">
-        <f>F601*B601+G601*(E588+$A$2*D601)</f>
-        <v>20715916.877506405</v>
+      <c r="E601" s="2">
+        <f>F601*B601+G601*(E588-$A$2*D601)</f>
+        <v>20717634.19425473</v>
       </c>
       <c r="F601" s="1">
         <f>IF(F588-$A$4 &lt;= $A$4,0.01,F588-$A$4)</f>
@@ -9102,11 +9103,11 @@
       </c>
       <c r="J601" s="1">
         <f>E601-E588</f>
-        <v>-16.333447135984898</v>
+        <v>34.010671630501747</v>
       </c>
       <c r="K601" s="1">
         <f>E601-B601</f>
-        <v>-1731.0934935957193</v>
+        <v>-13.776745270937681</v>
       </c>
     </row>
     <row r="602" spans="1:11" x14ac:dyDescent="0.25">
@@ -9268,9 +9269,9 @@
       <c r="D614" s="1">
         <v>-178.69399999999999</v>
       </c>
-      <c r="E614" s="1">
-        <f>F614*B614+G614*(E601+$A$2*D614)</f>
-        <v>20715900.875889942</v>
+      <c r="E614" s="2">
+        <f>F614*B614+G614*(E601-$A$2*D614)</f>
+        <v>20717668.296106376</v>
       </c>
       <c r="F614" s="1">
         <f>IF(F601-$A$4 &lt;= $A$4,0.01,F601-$A$4)</f>
@@ -9286,11 +9287,11 @@
       </c>
       <c r="J614" s="1">
         <f>E614-E601</f>
-        <v>-16.001616463065147</v>
+        <v>34.101851645857096</v>
       </c>
       <c r="K614" s="1">
         <f>E614-B614</f>
-        <v>-1777.074110057205</v>
+        <v>-9.6538936235010624</v>
       </c>
     </row>
     <row r="615" spans="1:11" x14ac:dyDescent="0.25">
@@ -9452,9 +9453,9 @@
       <c r="D627" s="1">
         <v>-178.54599999999999</v>
       </c>
-      <c r="E627" s="1">
-        <f>F627*B627+G627*(E614+$A$2*D627)</f>
-        <v>20715885.451858442</v>
+      <c r="E627" s="2">
+        <f>F627*B627+G627*(E614-$A$2*D627)</f>
+        <v>20717702.418787673</v>
       </c>
       <c r="F627" s="1">
         <f>IF(F614-$A$4 &lt;= $A$4,0.01,F614-$A$4)</f>
@@ -9470,11 +9471,11 @@
       </c>
       <c r="J627" s="1">
         <f>E627-E614</f>
-        <v>-15.424031499773264</v>
+        <v>34.122681297361851</v>
       </c>
       <c r="K627" s="1">
         <f>E627-B627</f>
-        <v>-1831.4711415581405</v>
+        <v>-14.504212327301502</v>
       </c>
     </row>
     <row r="628" spans="1:11" x14ac:dyDescent="0.25">
@@ -9636,9 +9637,9 @@
       <c r="D640" s="1">
         <v>-179.3</v>
       </c>
-      <c r="E640" s="1">
-        <f>F640*B640+G640*(E627+$A$2*D640)</f>
-        <v>20715870.259089857</v>
+      <c r="E640" s="2">
+        <f>F640*B640+G640*(E627-$A$2*D640)</f>
+        <v>20717736.561138771</v>
       </c>
       <c r="F640" s="1">
         <f>IF(F627-$A$4 &lt;= $A$4,0.01,F627-$A$4)</f>
@@ -9654,11 +9655,11 @@
       </c>
       <c r="J640" s="1">
         <f>E640-E627</f>
-        <v>-15.192768584936857</v>
+        <v>34.142351098358631</v>
       </c>
       <c r="K640" s="1">
         <f>E640-B640</f>
-        <v>-1868.5489101409912</v>
+        <v>-2.2468612268567085</v>
       </c>
     </row>
     <row r="641" spans="1:11" x14ac:dyDescent="0.25">
@@ -9820,9 +9821,9 @@
       <c r="D653" s="1">
         <v>-179.36799999999999</v>
       </c>
-      <c r="E653" s="1">
-        <f>F653*B653+G653*(E640+$A$2*D653)</f>
-        <v>20715855.676128156</v>
+      <c r="E653" s="2">
+        <f>F653*B653+G653*(E640-$A$2*D653)</f>
+        <v>20717770.845546931</v>
       </c>
       <c r="F653" s="1">
         <f>IF(F640-$A$4 &lt;= $A$4,0.01,F640-$A$4)</f>
@@ -9838,11 +9839,11 @@
       </c>
       <c r="J653" s="1">
         <f>E653-E640</f>
-        <v>-14.582961700856686</v>
+        <v>34.284408159554005</v>
       </c>
       <c r="K653" s="1">
         <f>E653-B653</f>
-        <v>-1930.1988718435168</v>
+        <v>-15.029453068971634</v>
       </c>
     </row>
     <row r="654" spans="1:11" x14ac:dyDescent="0.25">
@@ -10004,9 +10005,9 @@
       <c r="D666" s="1">
         <v>-180.57300000000001</v>
       </c>
-      <c r="E666" s="1">
-        <f>F666*B666+G666*(E653+$A$2*D666)</f>
-        <v>20715841.207205575</v>
+      <c r="E666" s="2">
+        <f>F666*B666+G666*(E653-$A$2*D666)</f>
+        <v>20717805.208991848</v>
       </c>
       <c r="F666" s="1">
         <f>IF(F653-$A$4 &lt;= $A$4,0.01,F653-$A$4)</f>
@@ -10022,11 +10023,11 @@
       </c>
       <c r="J666" s="1">
         <f>E666-E653</f>
-        <v>-14.468922581523657</v>
+        <v>34.363444916903973</v>
       </c>
       <c r="K666" s="1">
         <f>E666-B666</f>
-        <v>-1964.1547944247723</v>
+        <v>-0.15300815179944038</v>
       </c>
     </row>
     <row r="667" spans="1:11" x14ac:dyDescent="0.25">
@@ -10188,9 +10189,9 @@
       <c r="D679" s="1">
         <v>-182.64500000000001</v>
       </c>
-      <c r="E679" s="1">
-        <f>F679*B679+G679*(E666+$A$2*D679)</f>
-        <v>20715826.981889017</v>
+      <c r="E679" s="2">
+        <f>F679*B679+G679*(E666-$A$2*D679)</f>
+        <v>20717840.107807919</v>
       </c>
       <c r="F679" s="1">
         <f>IF(F666-$A$4 &lt;= $A$4,0.01,F666-$A$4)</f>
@@ -10206,11 +10207,11 @@
       </c>
       <c r="J679" s="1">
         <f>E679-E666</f>
-        <v>-14.225316558033228</v>
+        <v>34.89881607145071</v>
       </c>
       <c r="K679" s="1">
         <f>E679-B679</f>
-        <v>-2027.2461109831929</v>
+        <v>-14.12019208073616</v>
       </c>
     </row>
     <row r="680" spans="1:11" x14ac:dyDescent="0.25">
@@ -10372,9 +10373,9 @@
       <c r="D692" s="1">
         <v>-183.99799999999999</v>
       </c>
-      <c r="E692" s="1">
-        <f>F692*B692+G692*(E679+$A$2*D692)</f>
-        <v>20715812.950116325</v>
+      <c r="E692" s="2">
+        <f>F692*B692+G692*(E679-$A$2*D692)</f>
+        <v>20717875.218318496</v>
       </c>
       <c r="F692" s="1">
         <f>IF(F679-$A$4 &lt;= $A$4,0.01,F679-$A$4)</f>
@@ -10390,11 +10391,11 @@
       </c>
       <c r="J692" s="1">
         <f>E692-E679</f>
-        <v>-14.031772691756487</v>
+        <v>35.11051057651639</v>
       </c>
       <c r="K692" s="1">
         <f>E692-B692</f>
-        <v>-2071.85688367486</v>
+        <v>-9.5886815041303635</v>
       </c>
     </row>
     <row r="693" spans="1:11" x14ac:dyDescent="0.25">
@@ -10556,9 +10557,9 @@
       <c r="D705" s="1">
         <v>-184.05099999999999</v>
       </c>
-      <c r="E705" s="1">
-        <f>F705*B705+G705*(E692+$A$2*D705)</f>
-        <v>20715799.243552063</v>
+      <c r="E705" s="2">
+        <f>F705*B705+G705*(E692-$A$2*D705)</f>
+        <v>20717910.182568673</v>
       </c>
       <c r="F705" s="1">
         <f>IF(F692-$A$4 &lt;= $A$4,0.01,F692-$A$4)</f>
@@ -10574,11 +10575,11 @@
       </c>
       <c r="J705" s="1">
         <f>E705-E692</f>
-        <v>-13.706564262509346</v>
+        <v>34.964250177145004</v>
       </c>
       <c r="K705" s="1">
         <f>E705-B705</f>
-        <v>-2105.0494479387999</v>
+        <v>5.8895686715841293</v>
       </c>
     </row>
     <row r="706" spans="1:11" x14ac:dyDescent="0.25">
@@ -10740,9 +10741,9 @@
       <c r="D718" s="1">
         <v>-182.732</v>
       </c>
-      <c r="E718" s="1">
-        <f>F718*B718+G718*(E705+$A$2*D718)</f>
-        <v>20715786.284907341</v>
+      <c r="E718" s="2">
+        <f>F718*B718+G718*(E705-$A$2*D718)</f>
+        <v>20717944.911438972</v>
       </c>
       <c r="F718" s="1">
         <f>IF(F705-$A$4 &lt;= $A$4,0.01,F705-$A$4)</f>
@@ -10758,11 +10759,11 @@
       </c>
       <c r="J718" s="1">
         <f>E718-E705</f>
-        <v>-12.958644721657038</v>
+        <v>34.728870298713446</v>
       </c>
       <c r="K718" s="1">
         <f>E718-B718</f>
-        <v>-2154.2830926589668</v>
+        <v>4.3434389717876911</v>
       </c>
     </row>
     <row r="719" spans="1:11" x14ac:dyDescent="0.25">
@@ -10924,9 +10925,9 @@
       <c r="D731" s="1">
         <v>-181.91200000000001</v>
       </c>
-      <c r="E731" s="1">
-        <f>F731*B731+G731*(E718+$A$2*D731)</f>
-        <v>20715774.107751068</v>
+      <c r="E731" s="2">
+        <f>F731*B731+G731*(E718-$A$2*D731)</f>
+        <v>20717979.63620016</v>
       </c>
       <c r="F731" s="1">
         <f>IF(F718-$A$4 &lt;= $A$4,0.01,F718-$A$4)</f>
@@ -10942,11 +10943,11 @@
       </c>
       <c r="J731" s="1">
         <f>E731-E718</f>
-        <v>-12.177156273275614</v>
+        <v>34.724761188030243</v>
       </c>
       <c r="K731" s="1">
         <f>E731-B731</f>
-        <v>-2216.2262489311397</v>
+        <v>-10.69779983907938</v>
       </c>
     </row>
     <row r="732" spans="1:11" x14ac:dyDescent="0.25">
@@ -11108,9 +11109,9 @@
       <c r="D744" s="1">
         <v>-181.91200000000001</v>
       </c>
-      <c r="E744" s="1">
-        <f>F744*B744+G744*(E731+$A$2*D744)</f>
-        <v>20715762.421106357</v>
+      <c r="E744" s="2">
+        <f>F744*B744+G744*(E731-$A$2*D744)</f>
+        <v>20718014.382453736</v>
       </c>
       <c r="F744" s="1">
         <f>IF(F731-$A$4 &lt;= $A$4,0.01,F731-$A$4)</f>
@@ -11126,11 +11127,11 @@
       </c>
       <c r="J744" s="1">
         <f>E744-E731</f>
-        <v>-11.686644710600376</v>
+        <v>34.746253576129675</v>
       </c>
       <c r="K744" s="1">
         <f>E744-B744</f>
-        <v>-2264.7868936434388</v>
+        <v>-12.825546264648438</v>
       </c>
     </row>
     <row r="745" spans="1:11" x14ac:dyDescent="0.25">
@@ -11292,9 +11293,9 @@
       <c r="D757" s="1">
         <v>-183.083</v>
       </c>
-      <c r="E757" s="1">
-        <f>F757*B757+G757*(E744+$A$2*D757)</f>
-        <v>20715750.810942996</v>
+      <c r="E757" s="2">
+        <f>F757*B757+G757*(E744-$A$2*D757)</f>
+        <v>20718049.18173033</v>
       </c>
       <c r="F757" s="1">
         <f>IF(F744-$A$4 &lt;= $A$4,0.01,F744-$A$4)</f>
@@ -11310,11 +11311,11 @@
       </c>
       <c r="J757" s="1">
         <f>E757-E744</f>
-        <v>-11.610163360834122</v>
+        <v>34.79927659407258</v>
       </c>
       <c r="K757" s="1">
         <f>E757-B757</f>
-        <v>-2294.385057002306</v>
+        <v>3.9857303313910961</v>
       </c>
     </row>
     <row r="758" spans="1:11" x14ac:dyDescent="0.25">
@@ -11476,9 +11477,9 @@
       <c r="D770" s="1">
         <v>-184.90700000000001</v>
       </c>
-      <c r="E770" s="1">
-        <f>F770*B770+G770*(E757+$A$2*D770)</f>
-        <v>20715739.531396866</v>
+      <c r="E770" s="2">
+        <f>F770*B770+G770*(E757-$A$2*D770)</f>
+        <v>20718084.534248859</v>
       </c>
       <c r="F770" s="1">
         <f>IF(F757-$A$4 &lt;= $A$4,0.01,F757-$A$4)</f>
@@ -11494,11 +11495,11 @@
       </c>
       <c r="J770" s="1">
         <f>E770-E757</f>
-        <v>-11.27954613044858</v>
+        <v>35.352518528699875</v>
       </c>
       <c r="K770" s="1">
         <f>E770-B770</f>
-        <v>-2361.425603132695</v>
+        <v>-16.422751139849424</v>
       </c>
     </row>
     <row r="771" spans="1:11" x14ac:dyDescent="0.25">
@@ -11660,9 +11661,9 @@
       <c r="D783" s="1">
         <v>-185.976</v>
       </c>
-      <c r="E783" s="1">
-        <f>F783*B783+G783*(E770+$A$2*D783)</f>
-        <v>20715728.445377298</v>
+      <c r="E783" s="2">
+        <f>F783*B783+G783*(E770-$A$2*D783)</f>
+        <v>20718120.0164419</v>
       </c>
       <c r="F783" s="1">
         <f>IF(F770-$A$4 &lt;= $A$4,0.01,F770-$A$4)</f>
@@ -11678,11 +11679,11 @@
       </c>
       <c r="J783" s="1">
         <f>E783-E770</f>
-        <v>-11.086019568145275</v>
+        <v>35.482193041592836</v>
       </c>
       <c r="K783" s="1">
         <f>E783-B783</f>
-        <v>-2400.6926227025688</v>
+        <v>-9.1215580999851227</v>
       </c>
     </row>
     <row r="784" spans="1:11" x14ac:dyDescent="0.25">
@@ -11844,9 +11845,9 @@
       <c r="D796" s="1">
         <v>-186.79900000000001</v>
       </c>
-      <c r="E796" s="1">
-        <f>F796*B796+G796*(E783+$A$2*D796)</f>
-        <v>20715717.693151623</v>
+      <c r="E796" s="2">
+        <f>F796*B796+G796*(E783-$A$2*D796)</f>
+        <v>20718155.676598586</v>
       </c>
       <c r="F796" s="1">
         <f>IF(F783-$A$4 &lt;= $A$4,0.01,F783-$A$4)</f>
@@ -11862,11 +11863,11 @@
       </c>
       <c r="J796" s="1">
         <f>E796-E783</f>
-        <v>-10.752225674688816</v>
+        <v>35.660156685858965</v>
       </c>
       <c r="K796" s="1">
         <f>E796-B796</f>
-        <v>-2449.2188483774662</v>
+        <v>-11.235401414334774</v>
       </c>
     </row>
     <row r="797" spans="1:11" x14ac:dyDescent="0.25">
@@ -12028,9 +12029,9 @@
       <c r="D809" s="1">
         <v>-187.096</v>
       </c>
-      <c r="E809" s="1">
-        <f>F809*B809+G809*(E796+$A$2*D809)</f>
-        <v>20715707.151472509</v>
+      <c r="E809" s="2">
+        <f>F809*B809+G809*(E796-$A$2*D809)</f>
+        <v>20718191.194995757</v>
       </c>
       <c r="F809" s="1">
         <f>IF(F796-$A$4 &lt;= $A$4,0.01,F796-$A$4)</f>
@@ -12046,11 +12047,11 @@
       </c>
       <c r="J809" s="1">
         <f>E809-E796</f>
-        <v>-10.541679114103317</v>
+        <v>35.51839717105031</v>
       </c>
       <c r="K809" s="1">
         <f>E809-B809</f>
-        <v>-2475.649527490139</v>
+        <v>8.3939957581460476</v>
       </c>
     </row>
     <row r="810" spans="1:11" x14ac:dyDescent="0.25">
@@ -12212,9 +12213,9 @@
       <c r="D822" s="1">
         <v>-188.67500000000001</v>
       </c>
-      <c r="E822" s="1">
-        <f>F822*B822+G822*(E809+$A$2*D822)</f>
-        <v>20715696.942830279</v>
+      <c r="E822" s="2">
+        <f>F822*B822+G822*(E809-$A$2*D822)</f>
+        <v>20718227.180307925</v>
       </c>
       <c r="F822" s="1">
         <f>IF(F809-$A$4 &lt;= $A$4,0.01,F809-$A$4)</f>
@@ -12230,11 +12231,11 @@
       </c>
       <c r="J822" s="1">
         <f>E822-E809</f>
-        <v>-10.208642229437828</v>
+        <v>35.985312167555094</v>
       </c>
       <c r="K822" s="1">
         <f>E822-B822</f>
-        <v>-2538.3211697191</v>
+        <v>-8.0836920738220215</v>
       </c>
     </row>
     <row r="823" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>